<commit_message>
Caching devices of user in redis
</commit_message>
<xml_diff>
--- a/doc_build/redis-vars-topics.xlsx
+++ b/doc_build/redis-vars-topics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>gBridge Redis Documentation</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>QUERY, EXECUTE, SYNC, DISCONNECT</t>
+  </si>
+  <si>
+    <t>gbridge:u{userid}:devices</t>
+  </si>
+  <si>
+    <t>--- (simple SET/GET)</t>
+  </si>
+  <si>
+    <t>Array containing information about user's devices and their supported traits</t>
   </si>
 </sst>
 </file>
@@ -215,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -229,6 +238,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -509,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +575,7 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
@@ -579,7 +592,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
+      <c r="B11" s="7"/>
       <c r="C11" t="s">
         <v>10</v>
       </c>
@@ -594,7 +607,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
+      <c r="B12" s="7"/>
       <c r="C12" t="s">
         <v>16</v>
       </c>
@@ -609,7 +622,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C13" t="s">
@@ -623,7 +636,7 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
+      <c r="B14" s="7"/>
       <c r="C14" t="s">
         <v>38</v>
       </c>
@@ -634,83 +647,94 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.1</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>39</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>